<commit_message>
testing in excel sheet
</commit_message>
<xml_diff>
--- a/vfetch/vidhyasaagar/test.xlsx
+++ b/vfetch/vidhyasaagar/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/vfetch/vidhyasaagar/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/my_works/vfetch/vidhyasaagar/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>tesr</t>
   </si>
@@ -45,6 +45,15 @@
   </si>
   <si>
     <t>zs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THIS IS TEST </t>
+  </si>
+  <si>
+    <t>HOW ARE YOU</t>
+  </si>
+  <si>
+    <t>WHO IS THIS</t>
   </si>
 </sst>
 </file>
@@ -359,65 +368,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>

</xml_diff>